<commit_message>
Update All: Deploy Streamlit
</commit_message>
<xml_diff>
--- a/pages/chiphi.xlsx
+++ b/pages/chiphi.xlsx
@@ -16,9 +16,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,12 +60,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -969,6 +972,34 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Expense</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Đi ăn liên hoan</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Bonding</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>12313131</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>45652</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>AwD</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>